<commit_message>
Added finishing touches & re-did power systems.
Updated boost converter to buck-boost with I2C, made all power traces thicker, added aesthetics.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 3\Chem-E Car Team\McMaster_Chem-E_Car_23-24\Car_Circuitry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 4\Chem-E Car Team\McMaster_Chem-E_Car_24-25\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3519C40-5C62-4D9C-BA8E-67282E85E024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70D345BA-C029-4C99-AE6C-0F5281A9E5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{7C4C1D7A-DC8F-4684-AA7B-9C3498B008D7}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="16800" windowHeight="9760" xr2:uid="{D7797F30-3CB2-4BFA-A5C6-95BEC055E7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>Comment</t>
   </si>
@@ -59,19 +59,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>2604-3102</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>BAT_IN</t>
-  </si>
-  <si>
-    <t>26043102</t>
-  </si>
-  <si>
-    <t>MP3213DH-LF-P</t>
+    <t>TPS552892RYQR</t>
   </si>
   <si>
     <t>Integrated Circuit</t>
@@ -80,9 +68,6 @@
     <t>BOOST1</t>
   </si>
   <si>
-    <t>SOP65P490X110-9N</t>
-  </si>
-  <si>
     <t>TPS61023DRLT</t>
   </si>
   <si>
@@ -92,34 +77,25 @@
     <t>SOTFL50P160X60-6N</t>
   </si>
   <si>
-    <t>2.2 nF</t>
+    <t>100 nF</t>
   </si>
   <si>
     <t>Capacitor</t>
   </si>
   <si>
-    <t>C1, C12</t>
-  </si>
-  <si>
-    <t>CAPC2012X75N</t>
-  </si>
-  <si>
-    <t>CL21B222KBANNNC</t>
-  </si>
-  <si>
-    <t>10 nF</t>
-  </si>
-  <si>
-    <t>C2, C5, C6, C17</t>
-  </si>
-  <si>
-    <t>CL21B103KBANNNC</t>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>CAPC2012X95N</t>
+  </si>
+  <si>
+    <t>CL21B104KBCNNNC</t>
   </si>
   <si>
     <t>10 μF</t>
   </si>
   <si>
-    <t>C3, C7, C8, C14</t>
+    <t>C3, C4, C19</t>
   </si>
   <si>
     <t>CAPC2012X140N</t>
@@ -128,43 +104,85 @@
     <t>CL21B106KOQNNNE</t>
   </si>
   <si>
+    <t>82 nF</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>CAPC1005X55N</t>
+  </si>
+  <si>
+    <t>GRM155R61A823KA01D</t>
+  </si>
+  <si>
+    <t>24 nF</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>CAPC2013X94N</t>
+  </si>
+  <si>
+    <t>08051C243JAT2A</t>
+  </si>
+  <si>
     <t>4.7 μF</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CAPC2012X135N</t>
-  </si>
-  <si>
-    <t>CL21B475KOFNNNE</t>
-  </si>
-  <si>
-    <t>2.2 μF</t>
-  </si>
-  <si>
-    <t>C9, C10</t>
-  </si>
-  <si>
-    <t>CL21B225KAFNNWE</t>
-  </si>
-  <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t>C11, C13</t>
-  </si>
-  <si>
-    <t>CAPC2012X95N</t>
-  </si>
-  <si>
-    <t>CL21B104KBCNNNC</t>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>CAPC1608X80N</t>
+  </si>
+  <si>
+    <t>C1608X6S1C475K080AC</t>
+  </si>
+  <si>
+    <t>56 μF</t>
+  </si>
+  <si>
+    <t>Capacitor Polarised</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>16SVF82M</t>
+  </si>
+  <si>
+    <t>20SVPF56MX</t>
   </si>
   <si>
     <t>22 μF</t>
   </si>
   <si>
-    <t>C15, C16</t>
+    <t>C9, C15, C16, C17</t>
+  </si>
+  <si>
+    <t>CAPC3225X270N</t>
+  </si>
+  <si>
+    <t>GRM32ER61E226KE15K</t>
+  </si>
+  <si>
+    <t>C10, C11, C12, C18</t>
+  </si>
+  <si>
+    <t>CL05B104KA5NNNC</t>
+  </si>
+  <si>
+    <t>27 μF</t>
+  </si>
+  <si>
+    <t>C13, C14</t>
+  </si>
+  <si>
+    <t>25SVPF27MX</t>
+  </si>
+  <si>
+    <t>C20, C21</t>
   </si>
   <si>
     <t>CAPC3216X180N</t>
@@ -173,7 +191,22 @@
     <t>CL31B226KPHNNNE</t>
   </si>
   <si>
-    <t>SSA34HE3_A_I</t>
+    <t>B3B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 3POS 2.5MM</t>
+  </si>
+  <si>
+    <t>CND, SVO, TMP</t>
+  </si>
+  <si>
+    <t>FP-B3B-XH-A_LF_SN-MFG</t>
+  </si>
+  <si>
+    <t>CMP-17439-000014-3</t>
+  </si>
+  <si>
+    <t>SSB44-M3_5BT</t>
   </si>
   <si>
     <t>Schottky Diode</t>
@@ -182,10 +215,25 @@
     <t>D1</t>
   </si>
   <si>
-    <t>DIONM5127X229N</t>
-  </si>
-  <si>
-    <t>DRV8833PWPR</t>
+    <t>DIOM5436X244N</t>
+  </si>
+  <si>
+    <t>B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 2POS 2.5MM</t>
+  </si>
+  <si>
+    <t>DRML, DRMR, PROP, SOL, STMB, STMP, SW</t>
+  </si>
+  <si>
+    <t>FP-B2B-XH-A_LF_SN-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-05888-3</t>
+  </si>
+  <si>
+    <t>DRV8847PWPR</t>
   </si>
   <si>
     <t>DRV1, DRV2</t>
@@ -194,30 +242,6 @@
     <t>SOP65P640X120-17N</t>
   </si>
   <si>
-    <t>DRV8833PWP</t>
-  </si>
-  <si>
-    <t>B3B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 3POS 2.5MM</t>
-  </si>
-  <si>
-    <t>DS18B20_IN, SER0039_OUT</t>
-  </si>
-  <si>
-    <t>FP-B3B-XH-A_LF_SN-MFG</t>
-  </si>
-  <si>
-    <t>CMP-17439-000014-3</t>
-  </si>
-  <si>
-    <t>MPU6050</t>
-  </si>
-  <si>
-    <t>IMU</t>
-  </si>
-  <si>
     <t>4.7 μH</t>
   </si>
   <si>
@@ -227,10 +251,7 @@
     <t>L1</t>
   </si>
   <si>
-    <t>CDRH8D43NP4R7NC</t>
-  </si>
-  <si>
-    <t>CDRH8D43NP-4R7NC</t>
+    <t>74438357010</t>
   </si>
   <si>
     <t>1 μH</t>
@@ -239,25 +260,7 @@
     <t>L2</t>
   </si>
   <si>
-    <t>74438357010</t>
-  </si>
-  <si>
-    <t>B2B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 2POS 2.5MM</t>
-  </si>
-  <si>
-    <t>M1_OUT, M2_OUT, M3_OUT, M4_OUT, SW_IN</t>
-  </si>
-  <si>
-    <t>FP-B2B-XH-A_LF_SN-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2000-05888-3</t>
-  </si>
-  <si>
-    <t>Feather M0 Adalogger</t>
+    <t>Feather RP2040 Adalogger</t>
   </si>
   <si>
     <t>Adafruit Microcontroller</t>
@@ -269,112 +272,115 @@
     <t>2796</t>
   </si>
   <si>
-    <t>15 kΩ</t>
+    <t>DMN6075S-7</t>
+  </si>
+  <si>
+    <t>MOSFET (N-Channel)</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SOT96P240X110-3N</t>
+  </si>
+  <si>
+    <t>DMN6075SQ-7</t>
+  </si>
+  <si>
+    <t>110 mΩ</t>
   </si>
   <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RESC3216X70N</t>
-  </si>
-  <si>
-    <t>RMCF1206FT15K0</t>
+    <t>R1, R4</t>
+  </si>
+  <si>
+    <t>ERJ6_B_BW_R_LW_CW_D</t>
+  </si>
+  <si>
+    <t>ERJ-6DSFR11V</t>
+  </si>
+  <si>
+    <t>680 mΩ</t>
+  </si>
+  <si>
+    <t>R2, R5</t>
+  </si>
+  <si>
+    <t>ERJ-6DQJR68V</t>
   </si>
   <si>
     <t>10 kΩ</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RMCF1206FT10K0</t>
-  </si>
-  <si>
-    <t>75 kΩ</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>RESC3116X65N</t>
-  </si>
-  <si>
-    <t>RC1206FR-0775KL</t>
-  </si>
-  <si>
-    <t>2.2 kΩ</t>
-  </si>
-  <si>
-    <t>R4, R7</t>
-  </si>
-  <si>
-    <t>RESAD1042W49L330D178</t>
-  </si>
-  <si>
-    <t>RNMF14FTC2K20</t>
-  </si>
-  <si>
-    <t>180 mΩ</t>
-  </si>
-  <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>ERJ6_B_BW_R_LW_CW_D</t>
-  </si>
-  <si>
-    <t>ERJ-6DSFR18V</t>
-  </si>
-  <si>
-    <t>R6, R9</t>
+    <t>R3, R6</t>
+  </si>
+  <si>
+    <t>RESC2012X70N</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>RESC1005X40N</t>
+  </si>
+  <si>
+    <t>CRCW0402301RFKED</t>
+  </si>
+  <si>
+    <t>49.9 kΩ</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>ERJ2RKD1004X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF4992X</t>
+  </si>
+  <si>
+    <t>100 kΩ</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>ERJ8ENF1000V</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF1003V</t>
+  </si>
+  <si>
+    <t>732 kΩ</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF7323V</t>
   </si>
   <si>
     <t>4.7 kΩ</t>
   </si>
   <si>
-    <t>R10</t>
+    <t>R11</t>
   </si>
   <si>
     <t>RESAD1530W60L610D230</t>
   </si>
   <si>
     <t>CF1_4C472J</t>
-  </si>
-  <si>
-    <t>100 kΩ</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>ERJ8ENF1000V</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF1003V</t>
-  </si>
-  <si>
-    <t>732 kΩ</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF7323V</t>
-  </si>
-  <si>
-    <t>330 mΩ</t>
-  </si>
-  <si>
-    <t>ERJ-6DQFR33V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,9 +442,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{13495767-D579-47BC-AAED-6BB64B3CEC57}"/>
-  </tableStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -766,21 +770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D87CA4-DF68-481F-BB73-0AEC5228FBA2}">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF089C7-A640-47F8-B4A0-A2FA1AE2DDEE}">
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -814,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -825,19 +822,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -845,22 +842,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -868,39 +865,39 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -908,7 +905,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>26</v>
@@ -920,7 +917,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -928,7 +925,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
@@ -948,59 +945,59 @@
         <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1008,36 +1005,36 @@
         <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -1045,39 +1042,39 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1100,7 +1097,7 @@
         <v>63</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1108,7 +1105,7 @@
         <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>65</v>
@@ -1117,10 +1114,10 @@
         <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1137,27 +1134,27 @@
         <v>70</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1165,19 +1162,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1185,19 +1182,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1205,39 +1202,39 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1245,42 +1242,40 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1288,7 +1283,7 @@
         <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>98</v>
@@ -1308,7 +1303,7 @@
         <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>102</v>
@@ -1328,7 +1323,7 @@
         <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>106</v>
@@ -1343,8 +1338,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced conductivity probe port with backup servo port. Updated pin.
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 4\Chem-E Car Team\McMaster_Chem-E_Car_24-25\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70D345BA-C029-4C99-AE6C-0F5281A9E5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6EE28A4-8131-4FEA-BBBB-414C7C1B9DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="16800" windowHeight="9760" xr2:uid="{D7797F30-3CB2-4BFA-A5C6-95BEC055E7BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{18D7BE9C-05EF-4C69-953A-502343677836}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="113">
   <si>
     <t>Comment</t>
   </si>
@@ -191,190 +191,193 @@
     <t>CL31B226KPHNNNE</t>
   </si>
   <si>
+    <t>SSB44-M3_5BT</t>
+  </si>
+  <si>
+    <t>Schottky Diode</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DIOM5436X244N</t>
+  </si>
+  <si>
+    <t>B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 2POS 2.5MM</t>
+  </si>
+  <si>
+    <t>DRML, DRMR, PROP, SOL, STMB, STMP, SW</t>
+  </si>
+  <si>
+    <t>FP-B2B-XH-A_LF_SN-MFG</t>
+  </si>
+  <si>
+    <t>CMP-2000-05888-3</t>
+  </si>
+  <si>
+    <t>DRV8847PWPR</t>
+  </si>
+  <si>
+    <t>DRV1, DRV2</t>
+  </si>
+  <si>
+    <t>SOP65P640X120-17N</t>
+  </si>
+  <si>
+    <t>4.7 μH</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>74438357010</t>
+  </si>
+  <si>
+    <t>1 μH</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Feather RP2040 Adalogger</t>
+  </si>
+  <si>
+    <t>Adafruit Microcontroller</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>2796</t>
+  </si>
+  <si>
+    <t>DMN6075S-7</t>
+  </si>
+  <si>
+    <t>MOSFET (N-Channel)</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SOT96P240X110-3N</t>
+  </si>
+  <si>
+    <t>DMN6075SQ-7</t>
+  </si>
+  <si>
+    <t>110 mΩ</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R1, R4</t>
+  </si>
+  <si>
+    <t>ERJ6_B_BW_R_LW_CW_D</t>
+  </si>
+  <si>
+    <t>ERJ-6DSFR11V</t>
+  </si>
+  <si>
+    <t>680 mΩ</t>
+  </si>
+  <si>
+    <t>R2, R5</t>
+  </si>
+  <si>
+    <t>ERJ-6DQJR68V</t>
+  </si>
+  <si>
+    <t>10 kΩ</t>
+  </si>
+  <si>
+    <t>R3, R6</t>
+  </si>
+  <si>
+    <t>RESC2012X70N</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ103V</t>
+  </si>
+  <si>
+    <t>4.7 kΩ</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>RESAD1530W60L610D230</t>
+  </si>
+  <si>
+    <t>CF1_4C472J</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>RESC1005X40N</t>
+  </si>
+  <si>
+    <t>CRCW0402301RFKED</t>
+  </si>
+  <si>
+    <t>49.9 kΩ</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>ERJ2RKD1004X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF4992X</t>
+  </si>
+  <si>
+    <t>100 kΩ</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>ERJ8ENF1000V</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF1003V</t>
+  </si>
+  <si>
+    <t>732 kΩ</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ERJ-8ENF7323V</t>
+  </si>
+  <si>
     <t>B3B-XH-A(LF)(SN)</t>
   </si>
   <si>
     <t>CONN HEADER VERT 3POS 2.5MM</t>
   </si>
   <si>
-    <t>CND, SVO, TMP</t>
+    <t>SVOB, SVOP, TMP</t>
   </si>
   <si>
     <t>FP-B3B-XH-A_LF_SN-MFG</t>
   </si>
   <si>
     <t>CMP-17439-000014-3</t>
-  </si>
-  <si>
-    <t>SSB44-M3_5BT</t>
-  </si>
-  <si>
-    <t>Schottky Diode</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>DIOM5436X244N</t>
-  </si>
-  <si>
-    <t>B2B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 2POS 2.5MM</t>
-  </si>
-  <si>
-    <t>DRML, DRMR, PROP, SOL, STMB, STMP, SW</t>
-  </si>
-  <si>
-    <t>FP-B2B-XH-A_LF_SN-MFG</t>
-  </si>
-  <si>
-    <t>CMP-2000-05888-3</t>
-  </si>
-  <si>
-    <t>DRV8847PWPR</t>
-  </si>
-  <si>
-    <t>DRV1, DRV2</t>
-  </si>
-  <si>
-    <t>SOP65P640X120-17N</t>
-  </si>
-  <si>
-    <t>4.7 μH</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>74438357010</t>
-  </si>
-  <si>
-    <t>1 μH</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>Feather RP2040 Adalogger</t>
-  </si>
-  <si>
-    <t>Adafruit Microcontroller</t>
-  </si>
-  <si>
-    <t>MCU</t>
-  </si>
-  <si>
-    <t>2796</t>
-  </si>
-  <si>
-    <t>DMN6075S-7</t>
-  </si>
-  <si>
-    <t>MOSFET (N-Channel)</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SOT96P240X110-3N</t>
-  </si>
-  <si>
-    <t>DMN6075SQ-7</t>
-  </si>
-  <si>
-    <t>110 mΩ</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R1, R4</t>
-  </si>
-  <si>
-    <t>ERJ6_B_BW_R_LW_CW_D</t>
-  </si>
-  <si>
-    <t>ERJ-6DSFR11V</t>
-  </si>
-  <si>
-    <t>680 mΩ</t>
-  </si>
-  <si>
-    <t>R2, R5</t>
-  </si>
-  <si>
-    <t>ERJ-6DQJR68V</t>
-  </si>
-  <si>
-    <t>10 kΩ</t>
-  </si>
-  <si>
-    <t>R3, R6</t>
-  </si>
-  <si>
-    <t>RESC2012X70N</t>
-  </si>
-  <si>
-    <t>ERJ-6GEYJ103V</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>RESC1005X40N</t>
-  </si>
-  <si>
-    <t>CRCW0402301RFKED</t>
-  </si>
-  <si>
-    <t>49.9 kΩ</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>ERJ2RKD1004X</t>
-  </si>
-  <si>
-    <t>ERJ-2RKF4992X</t>
-  </si>
-  <si>
-    <t>100 kΩ</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>ERJ8ENF1000V</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF1003V</t>
-  </si>
-  <si>
-    <t>732 kΩ</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>ERJ-8ENF7323V</t>
-  </si>
-  <si>
-    <t>4.7 kΩ</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>RESAD1530W60L610D230</t>
-  </si>
-  <si>
-    <t>CF1_4C472J</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF089C7-A640-47F8-B4A0-A2FA1AE2DDEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8325990-4E2A-4925-AAC5-D6BA8CE178F2}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1054,30 +1057,30 @@
         <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F15" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1085,56 +1088,56 @@
         <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F16" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -1142,19 +1145,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -1162,16 +1165,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>76</v>
@@ -1197,7 +1200,7 @@
         <v>81</v>
       </c>
       <c r="F21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1205,16 +1208,16 @@
         <v>82</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
@@ -1222,19 +1225,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1242,28 +1245,30 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>94</v>
@@ -1283,7 +1288,7 @@
         <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>98</v>
@@ -1303,7 +1308,7 @@
         <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>102</v>
@@ -1323,7 +1328,7 @@
         <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>106</v>
@@ -1343,19 +1348,19 @@
         <v>108</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update bom & things
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 4\Chem-E Car Team\McMaster_Chem-E_Car_24-25\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6EE28A4-8131-4FEA-BBBB-414C7C1B9DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A92F731-4958-43C5-BAE5-85D435618DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{18D7BE9C-05EF-4C69-953A-502343677836}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{05918D5E-7A5B-4C8F-A5B8-37F9F4E5FD1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
     <t>10 kΩ</t>
   </si>
   <si>
-    <t>R3, R6</t>
+    <t>R3, R6, R10</t>
   </si>
   <si>
     <t>RESC2012X70N</t>
@@ -320,7 +320,7 @@
     <t>CF1_4C472J</t>
   </si>
   <si>
-    <t/>
+    <t>301 Ω</t>
   </si>
   <si>
     <t>R8</t>
@@ -347,7 +347,7 @@
     <t>100 kΩ</t>
   </si>
   <si>
-    <t>R10</t>
+    <t>R11</t>
   </si>
   <si>
     <t>ERJ8ENF1000V</t>
@@ -359,7 +359,7 @@
     <t>732 kΩ</t>
   </si>
   <si>
-    <t>R11</t>
+    <t>R12</t>
   </si>
   <si>
     <t>ERJ-8ENF7323V</t>
@@ -773,7 +773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8325990-4E2A-4925-AAC5-D6BA8CE178F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94739D9-93EE-436C-AD48-E7FE6C927A0E}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1240,7 +1240,7 @@
         <v>88</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fixed messed up inductor & updated bom
</commit_message>
<xml_diff>
--- a/Car_Circuitry/Car_Circuitry_BOM.xlsx
+++ b/Car_Circuitry/Car_Circuitry_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oasis\Documents\School\Assignments\Undergraduate Year 4\Chem-E Car Team\McMaster_Chem-E_Car_24-25\Car_Circuitry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A92F731-4958-43C5-BAE5-85D435618DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93615B8E-6D8F-43D1-B40E-494881BD6175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{05918D5E-7A5B-4C8F-A5B8-37F9F4E5FD1E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{E830964A-B488-45D9-84B5-630F87D382AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Circuitry_BOM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
   <si>
     <t>Comment</t>
   </si>
@@ -236,15 +236,21 @@
     <t>L1</t>
   </si>
   <si>
+    <t>INDPM6664X610N</t>
+  </si>
+  <si>
+    <t>74439346047</t>
+  </si>
+  <si>
+    <t>1 μH</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
     <t>74438357010</t>
   </si>
   <si>
-    <t>1 μH</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>Feather RP2040 Adalogger</t>
   </si>
   <si>
@@ -378,12 +384,18 @@
   </si>
   <si>
     <t>CMP-17439-000014-3</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Boards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,7 +457,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{0EF9EE6F-4735-4533-8222-9EDEA1268861}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -773,17 +787,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94739D9-93EE-436C-AD48-E7FE6C927A0E}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F29A72-50C2-4BC0-A284-E1CCECBBF6C2}">
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -802,8 +818,14 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -822,8 +844,15 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1">
+        <f>F2*$H$2</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -842,8 +871,12 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G29" si="0">F3*$H$2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -862,8 +895,12 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -882,8 +919,12 @@
       <c r="F5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -902,8 +943,12 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -922,8 +967,12 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -942,8 +991,12 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -962,8 +1015,12 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -982,8 +1039,12 @@
       <c r="F10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1002,8 +1063,12 @@
       <c r="F11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1022,8 +1087,12 @@
       <c r="F12" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1042,8 +1111,12 @@
       <c r="F13" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -1062,8 +1135,12 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -1082,8 +1159,12 @@
       <c r="F15" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1102,8 +1183,12 @@
       <c r="F16" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -1117,250 +1202,302 @@
         <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F23" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F29" s="1">
         <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>